<commit_message>
Release 1.1 - Update components values + BOM - Update of J1 pins affectation now matching J2 distribution. - Update gerber files with missing inner layers - Few updates of the PCB layout (J2 redraw + decoupling cap)
</commit_message>
<xml_diff>
--- a/hardware/udriver3/uOmodri_BOM.xlsx
+++ b/hardware/udriver3/uOmodri_BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20368"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20378"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmanhes\LAAS\Actionneur\OMODRI\hardware\udriver3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54FBEDC8-45BA-45FF-A227-83AE86DFF9AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE01C2F-7C30-4C1D-AB27-192B2906D07E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11925" xr2:uid="{800813FF-B8B0-4030-B776-D6B1FB122AF2}"/>
   </bookViews>
@@ -1349,7 +1349,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A59EB06-C53C-4109-98AE-B18B33EAFA36}">
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -2563,7 +2563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>153</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>272</v>
       </c>
@@ -2766,7 +2766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>273</v>
       </c>
@@ -2882,7 +2882,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>197</v>
       </c>

</xml_diff>